<commit_message>
changes in html and py for expense
</commit_message>
<xml_diff>
--- a/static/excels/Expenses02.xlsx
+++ b/static/excels/Expenses02.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
-  <si>
-    <t>Ledger Report of AK</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+  <si>
+    <t>Ledger Report of muku</t>
   </si>
   <si>
     <t>Date</t>
@@ -40,58 +40,28 @@
     <t>Received</t>
   </si>
   <si>
-    <t>16-11-2018</t>
-  </si>
-  <si>
-    <t>Strawberry</t>
+    <t>20-01-2020</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>27-01-2020</t>
+  </si>
+  <si>
+    <t>sitaphal</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>15-11-2018</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>19-11-2018</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>30-11-2018</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>03-12-2018</t>
-  </si>
-  <si>
-    <t>04-12-2018</t>
-  </si>
-  <si>
-    <t>03/10/2018</t>
-  </si>
-  <si>
-    <t>09-10-2018</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>20-11-2018</t>
+    <t>13-01-2020</t>
+  </si>
+  <si>
+    <t>28-01-2020</t>
   </si>
   <si>
     <t>Remaining Balance</t>
@@ -435,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D2:J17"/>
+  <dimension ref="D2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,16 +450,16 @@
         <v>10</v>
       </c>
       <c r="G6">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>5600</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="4:10">
@@ -503,16 +473,16 @@
         <v>13</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J7">
-        <v>4000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="4:10">
@@ -523,211 +493,50 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G8">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>380</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>31920</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="4:10">
       <c r="D9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10">
+      <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G9">
-        <v>80</v>
-      </c>
-      <c r="H9">
-        <v>395</v>
-      </c>
-      <c r="I9">
-        <v>31600</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10">
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10">
-        <v>63</v>
-      </c>
-      <c r="H10">
-        <v>400</v>
-      </c>
-      <c r="I10">
-        <v>25200</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10">
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11">
-        <v>28</v>
-      </c>
-      <c r="H11">
-        <v>320</v>
-      </c>
-      <c r="I11">
-        <v>8960</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="4:10">
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12">
-        <v>14</v>
-      </c>
-      <c r="H12">
-        <v>230</v>
-      </c>
-      <c r="I12">
-        <v>3220</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="4:10">
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>14</v>
-      </c>
-      <c r="H13">
-        <v>400</v>
-      </c>
-      <c r="I13">
-        <v>5600</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="4:10">
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14">
-        <v>28</v>
-      </c>
-      <c r="H14">
-        <v>400</v>
-      </c>
-      <c r="I14">
-        <v>11200</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="4:10">
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15">
-        <v>7</v>
-      </c>
-      <c r="H15">
-        <v>380</v>
-      </c>
-      <c r="I15">
-        <v>2660</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="4:10">
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="17" spans="4:9">
-      <c r="D17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="1">
-        <v>46280</v>
+      <c r="I10" s="1">
+        <v>11612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>